<commit_message>
correct impl nf (&slow)
</commit_message>
<xml_diff>
--- a/results/nf/15x15/all/nf_all_15x15_True_2.xlsx
+++ b/results/nf/15x15/all/nf_all_15x15_True_2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -483,16 +483,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00353</v>
+        <v>0.31581</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00177</v>
+        <v>0.15791</v>
       </c>
       <c r="F2" t="n">
-        <v>0.22162</v>
+        <v>15.15159</v>
       </c>
       <c r="G2" t="n">
         <v>0.85</v>
@@ -509,16 +509,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00222</v>
+        <v>0.41622</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00111</v>
+        <v>0.20811</v>
       </c>
       <c r="F3" t="n">
-        <v>0.13259</v>
+        <v>14.60238</v>
       </c>
       <c r="G3" t="n">
         <v>0.85</v>
@@ -535,16 +535,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00178</v>
+        <v>0.18732</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0008899999999999999</v>
+        <v>0.09365999999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0.09261</v>
+        <v>11.42057</v>
       </c>
       <c r="G4" t="n">
         <v>0.85</v>
@@ -561,16 +561,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0022</v>
+        <v>0.38842</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0011</v>
+        <v>0.19421</v>
       </c>
       <c r="F5" t="n">
-        <v>0.11158</v>
+        <v>19.60782</v>
       </c>
       <c r="G5" t="n">
         <v>0.85</v>
@@ -587,16 +587,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00247</v>
+        <v>0.37863</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00124</v>
+        <v>0.18932</v>
       </c>
       <c r="F6" t="n">
-        <v>0.13561</v>
+        <v>17.34374</v>
       </c>
       <c r="G6" t="n">
         <v>0.85</v>
@@ -613,16 +613,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00293</v>
+        <v>0.24488</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00146</v>
+        <v>0.12244</v>
       </c>
       <c r="F7" t="n">
-        <v>0.16606</v>
+        <v>12.4012</v>
       </c>
       <c r="G7" t="n">
         <v>0.85</v>
@@ -639,16 +639,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00299</v>
+        <v>0.20341</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0015</v>
+        <v>0.1017</v>
       </c>
       <c r="F8" t="n">
-        <v>0.17958</v>
+        <v>12.22259</v>
       </c>
       <c r="G8" t="n">
         <v>0.85</v>
@@ -665,16 +665,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00284</v>
+        <v>0.31052</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00142</v>
+        <v>0.15526</v>
       </c>
       <c r="F9" t="n">
-        <v>0.18023</v>
+        <v>16.21818</v>
       </c>
       <c r="G9" t="n">
         <v>0.85</v>
@@ -691,16 +691,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00206</v>
+        <v>0.2047</v>
       </c>
       <c r="E10" t="n">
-        <v>0.00103</v>
+        <v>0.10235</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08962000000000001</v>
+        <v>15.06262</v>
       </c>
       <c r="G10" t="n">
         <v>0.85</v>
@@ -717,16 +717,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00143</v>
+        <v>0.23225</v>
       </c>
       <c r="E11" t="n">
-        <v>0.00072</v>
+        <v>0.11613</v>
       </c>
       <c r="F11" t="n">
-        <v>0.06849</v>
+        <v>15.01165</v>
       </c>
       <c r="G11" t="n">
         <v>0.85</v>
@@ -743,16 +743,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00216</v>
+        <v>0.25694</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00108</v>
+        <v>0.12847</v>
       </c>
       <c r="F12" t="n">
-        <v>0.11315</v>
+        <v>11.90626</v>
       </c>
       <c r="G12" t="n">
         <v>0.85</v>
@@ -769,16 +769,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00226</v>
+        <v>0.26786</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00113</v>
+        <v>0.13393</v>
       </c>
       <c r="F13" t="n">
-        <v>0.14522</v>
+        <v>13.15362</v>
       </c>
       <c r="G13" t="n">
         <v>0.85</v>
@@ -795,16 +795,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00206</v>
+        <v>0.25436</v>
       </c>
       <c r="E14" t="n">
-        <v>0.00103</v>
+        <v>0.12718</v>
       </c>
       <c r="F14" t="n">
-        <v>0.14223</v>
+        <v>15.61802</v>
       </c>
       <c r="G14" t="n">
         <v>0.85</v>
@@ -821,16 +821,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00243</v>
+        <v>0.39699</v>
       </c>
       <c r="E15" t="n">
-        <v>0.00122</v>
+        <v>0.19849</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1232</v>
+        <v>21.70678</v>
       </c>
       <c r="G15" t="n">
         <v>0.85</v>
@@ -847,16 +847,16 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D16" t="n">
-        <v>0.00232</v>
+        <v>0.28294</v>
       </c>
       <c r="E16" t="n">
-        <v>0.00116</v>
+        <v>0.14147</v>
       </c>
       <c r="F16" t="n">
-        <v>0.11752</v>
+        <v>15.6122</v>
       </c>
       <c r="G16" t="n">
         <v>0.85</v>
@@ -873,16 +873,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00207</v>
+        <v>0.44832</v>
       </c>
       <c r="E17" t="n">
-        <v>0.00103</v>
+        <v>0.22416</v>
       </c>
       <c r="F17" t="n">
-        <v>0.10951</v>
+        <v>15.7178</v>
       </c>
       <c r="G17" t="n">
         <v>0.85</v>
@@ -899,16 +899,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00259</v>
+        <v>0.23512</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00129</v>
+        <v>0.11756</v>
       </c>
       <c r="F18" t="n">
-        <v>0.15052</v>
+        <v>13.47016</v>
       </c>
       <c r="G18" t="n">
         <v>0.85</v>
@@ -925,16 +925,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D19" t="n">
-        <v>0.00215</v>
+        <v>0.47001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00107</v>
+        <v>0.23501</v>
       </c>
       <c r="F19" t="n">
-        <v>0.11761</v>
+        <v>17.75768</v>
       </c>
       <c r="G19" t="n">
         <v>0.85</v>
@@ -951,16 +951,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D20" t="n">
-        <v>0.00195</v>
+        <v>0.25411</v>
       </c>
       <c r="E20" t="n">
-        <v>0.00098</v>
+        <v>0.12706</v>
       </c>
       <c r="F20" t="n">
-        <v>0.10258</v>
+        <v>16.58328</v>
       </c>
       <c r="G20" t="n">
         <v>0.85</v>
@@ -977,16 +977,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002</v>
+        <v>0.40117</v>
       </c>
       <c r="E21" t="n">
-        <v>0.001</v>
+        <v>0.20058</v>
       </c>
       <c r="F21" t="n">
-        <v>0.11498</v>
+        <v>15.79928</v>
       </c>
       <c r="G21" t="n">
         <v>0.85</v>
@@ -1003,16 +1003,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0025</v>
+        <v>0.46282</v>
       </c>
       <c r="E22" t="n">
-        <v>0.00125</v>
+        <v>0.23141</v>
       </c>
       <c r="F22" t="n">
-        <v>0.10053</v>
+        <v>14.80198</v>
       </c>
       <c r="G22" t="n">
         <v>0.15</v>
@@ -1029,16 +1029,16 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00196</v>
+        <v>0.54127</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00098</v>
+        <v>0.27064</v>
       </c>
       <c r="F23" t="n">
-        <v>0.08461</v>
+        <v>17.59006</v>
       </c>
       <c r="G23" t="n">
         <v>0.15</v>
@@ -1055,16 +1055,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00224</v>
+        <v>0.34955</v>
       </c>
       <c r="E24" t="n">
-        <v>0.00112</v>
+        <v>0.17478</v>
       </c>
       <c r="F24" t="n">
-        <v>0.08051</v>
+        <v>12.84698</v>
       </c>
       <c r="G24" t="n">
         <v>0.15</v>
@@ -1081,16 +1081,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25" t="n">
-        <v>0.00274</v>
+        <v>0.44106</v>
       </c>
       <c r="E25" t="n">
-        <v>0.00137</v>
+        <v>0.22053</v>
       </c>
       <c r="F25" t="n">
-        <v>0.10052</v>
+        <v>15.56648</v>
       </c>
       <c r="G25" t="n">
         <v>0.15</v>
@@ -1107,16 +1107,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D26" t="n">
-        <v>0.00196</v>
+        <v>0.40265</v>
       </c>
       <c r="E26" t="n">
-        <v>0.00098</v>
+        <v>0.20132</v>
       </c>
       <c r="F26" t="n">
-        <v>0.05498</v>
+        <v>16.45278</v>
       </c>
       <c r="G26" t="n">
         <v>0.15</v>
@@ -1133,16 +1133,16 @@
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0034</v>
+        <v>0.19102</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0017</v>
+        <v>0.09551</v>
       </c>
       <c r="F27" t="n">
-        <v>0.13986</v>
+        <v>5.49707</v>
       </c>
       <c r="G27" t="n">
         <v>0.15</v>
@@ -1159,16 +1159,16 @@
         <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00266</v>
+        <v>0.32663</v>
       </c>
       <c r="E28" t="n">
-        <v>0.00133</v>
+        <v>0.16332</v>
       </c>
       <c r="F28" t="n">
-        <v>0.07976</v>
+        <v>11.42449</v>
       </c>
       <c r="G28" t="n">
         <v>0.15</v>
@@ -1185,16 +1185,16 @@
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D29" t="n">
-        <v>0.00181</v>
+        <v>0.29973</v>
       </c>
       <c r="E29" t="n">
-        <v>0.00091</v>
+        <v>0.14987</v>
       </c>
       <c r="F29" t="n">
-        <v>0.052</v>
+        <v>9.301119999999999</v>
       </c>
       <c r="G29" t="n">
         <v>0.15</v>
@@ -1211,16 +1211,16 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D30" t="n">
-        <v>0.00288</v>
+        <v>0.20236</v>
       </c>
       <c r="E30" t="n">
-        <v>0.00144</v>
+        <v>0.10118</v>
       </c>
       <c r="F30" t="n">
-        <v>0.08652</v>
+        <v>8.64629</v>
       </c>
       <c r="G30" t="n">
         <v>0.15</v>
@@ -1237,16 +1237,16 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D31" t="n">
-        <v>0.00206</v>
+        <v>0.25242</v>
       </c>
       <c r="E31" t="n">
-        <v>0.00103</v>
+        <v>0.12621</v>
       </c>
       <c r="F31" t="n">
-        <v>0.05652</v>
+        <v>7.74908</v>
       </c>
       <c r="G31" t="n">
         <v>0.15</v>
@@ -1263,16 +1263,16 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D32" t="n">
-        <v>0.00211</v>
+        <v>0.26013</v>
       </c>
       <c r="E32" t="n">
-        <v>0.00106</v>
+        <v>0.13007</v>
       </c>
       <c r="F32" t="n">
-        <v>0.06428</v>
+        <v>9.766360000000001</v>
       </c>
       <c r="G32" t="n">
         <v>0.15</v>
@@ -1289,16 +1289,16 @@
         <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>0.00207</v>
+        <v>0.3538</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00104</v>
+        <v>0.1769</v>
       </c>
       <c r="F33" t="n">
-        <v>0.07658</v>
+        <v>12.31556</v>
       </c>
       <c r="G33" t="n">
         <v>0.15</v>
@@ -1315,16 +1315,16 @@
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0016</v>
+        <v>0.48358</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0008</v>
+        <v>0.24179</v>
       </c>
       <c r="F34" t="n">
-        <v>0.05164</v>
+        <v>19.81099</v>
       </c>
       <c r="G34" t="n">
         <v>0.15</v>
@@ -1341,16 +1341,16 @@
         <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D35" t="n">
-        <v>0.00246</v>
+        <v>0.3958</v>
       </c>
       <c r="E35" t="n">
-        <v>0.00123</v>
+        <v>0.1979</v>
       </c>
       <c r="F35" t="n">
-        <v>0.08558</v>
+        <v>12.85913</v>
       </c>
       <c r="G35" t="n">
         <v>0.15</v>
@@ -1367,16 +1367,16 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0031</v>
+        <v>0.32942</v>
       </c>
       <c r="E36" t="n">
-        <v>0.00155</v>
+        <v>0.16471</v>
       </c>
       <c r="F36" t="n">
-        <v>0.10231</v>
+        <v>10.84931</v>
       </c>
       <c r="G36" t="n">
         <v>0.15</v>
@@ -1393,16 +1393,16 @@
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00188</v>
+        <v>0.17875</v>
       </c>
       <c r="E37" t="n">
-        <v>0.00094</v>
+        <v>0.08937</v>
       </c>
       <c r="F37" t="n">
-        <v>0.06807000000000001</v>
+        <v>6.51194</v>
       </c>
       <c r="G37" t="n">
         <v>0.15</v>
@@ -1419,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D38" t="n">
-        <v>0.00257</v>
+        <v>0.23396</v>
       </c>
       <c r="E38" t="n">
-        <v>0.00129</v>
+        <v>0.11698</v>
       </c>
       <c r="F38" t="n">
-        <v>0.08464000000000001</v>
+        <v>7.18161</v>
       </c>
       <c r="G38" t="n">
         <v>0.15</v>
@@ -1445,16 +1445,16 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D39" t="n">
-        <v>0.00247</v>
+        <v>0.29286</v>
       </c>
       <c r="E39" t="n">
-        <v>0.00124</v>
+        <v>0.14643</v>
       </c>
       <c r="F39" t="n">
-        <v>0.08461</v>
+        <v>9.06115</v>
       </c>
       <c r="G39" t="n">
         <v>0.15</v>
@@ -1471,16 +1471,16 @@
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D40" t="n">
-        <v>0.00219</v>
+        <v>0.24267</v>
       </c>
       <c r="E40" t="n">
-        <v>0.00109</v>
+        <v>0.12133</v>
       </c>
       <c r="F40" t="n">
-        <v>0.07962</v>
+        <v>6.75077</v>
       </c>
       <c r="G40" t="n">
         <v>0.15</v>
@@ -1497,16 +1497,16 @@
         <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D41" t="n">
-        <v>0.00184</v>
+        <v>0.38491</v>
       </c>
       <c r="E41" t="n">
-        <v>0.00092</v>
+        <v>0.19246</v>
       </c>
       <c r="F41" t="n">
-        <v>0.05901</v>
+        <v>11.59903</v>
       </c>
       <c r="G41" t="n">
         <v>0.15</v>
@@ -1523,19 +1523,19 @@
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00497</v>
+        <v>0.74822</v>
       </c>
       <c r="E42" t="n">
-        <v>0.00124</v>
+        <v>0.18706</v>
       </c>
       <c r="F42" t="n">
-        <v>0.18703</v>
+        <v>14.59911</v>
       </c>
       <c r="G42" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -1549,19 +1549,19 @@
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D43" t="n">
-        <v>0.00911</v>
+        <v>0.55346</v>
       </c>
       <c r="E43" t="n">
-        <v>0.00228</v>
+        <v>0.13837</v>
       </c>
       <c r="F43" t="n">
-        <v>0.32503</v>
+        <v>11.58555</v>
       </c>
       <c r="G43" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H43" t="n">
         <v>1</v>
@@ -1575,19 +1575,19 @@
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D44" t="n">
-        <v>0.006</v>
+        <v>0.58158</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0015</v>
+        <v>0.14539</v>
       </c>
       <c r="F44" t="n">
-        <v>0.23306</v>
+        <v>13.55854</v>
       </c>
       <c r="G44" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H44" t="n">
         <v>2</v>
@@ -1601,19 +1601,19 @@
         <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D45" t="n">
-        <v>0.00479</v>
+        <v>0.83606</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0012</v>
+        <v>0.20901</v>
       </c>
       <c r="F45" t="n">
-        <v>0.15159</v>
+        <v>20.03914</v>
       </c>
       <c r="G45" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H45" t="n">
         <v>3</v>
@@ -1627,19 +1627,19 @@
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D46" t="n">
-        <v>0.00435</v>
+        <v>1.12607</v>
       </c>
       <c r="E46" t="n">
-        <v>0.00109</v>
+        <v>0.28152</v>
       </c>
       <c r="F46" t="n">
-        <v>0.11164</v>
+        <v>21.12238</v>
       </c>
       <c r="G46" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H46" t="n">
         <v>4</v>
@@ -1653,19 +1653,19 @@
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D47" t="n">
-        <v>0.00438</v>
+        <v>0.64429</v>
       </c>
       <c r="E47" t="n">
-        <v>0.00109</v>
+        <v>0.16107</v>
       </c>
       <c r="F47" t="n">
-        <v>0.14745</v>
+        <v>14.80168</v>
       </c>
       <c r="G47" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H47" t="n">
         <v>5</v>
@@ -1679,19 +1679,19 @@
         <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D48" t="n">
-        <v>0.00773</v>
+        <v>0.39466</v>
       </c>
       <c r="E48" t="n">
-        <v>0.00193</v>
+        <v>0.09866999999999999</v>
       </c>
       <c r="F48" t="n">
-        <v>0.27657</v>
+        <v>8.282920000000001</v>
       </c>
       <c r="G48" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H48" t="n">
         <v>6</v>
@@ -1705,19 +1705,19 @@
         <v>1</v>
       </c>
       <c r="C49" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D49" t="n">
-        <v>0.00628</v>
+        <v>0.5033</v>
       </c>
       <c r="E49" t="n">
-        <v>0.00157</v>
+        <v>0.12583</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1861</v>
+        <v>12.734</v>
       </c>
       <c r="G49" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H49" t="n">
         <v>7</v>
@@ -1731,19 +1731,19 @@
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D50" t="n">
-        <v>0.00623</v>
+        <v>0.6137899999999999</v>
       </c>
       <c r="E50" t="n">
-        <v>0.00156</v>
+        <v>0.15345</v>
       </c>
       <c r="F50" t="n">
-        <v>0.19912</v>
+        <v>11.92961</v>
       </c>
       <c r="G50" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H50" t="n">
         <v>8</v>
@@ -1757,19 +1757,19 @@
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D51" t="n">
-        <v>0.00658</v>
+        <v>0.50337</v>
       </c>
       <c r="E51" t="n">
-        <v>0.00165</v>
+        <v>0.12584</v>
       </c>
       <c r="F51" t="n">
-        <v>0.38037</v>
+        <v>11.75516</v>
       </c>
       <c r="G51" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H51" t="n">
         <v>9</v>
@@ -1783,19 +1783,19 @@
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D52" t="n">
-        <v>0.00498</v>
+        <v>0.5347499999999999</v>
       </c>
       <c r="E52" t="n">
-        <v>0.00125</v>
+        <v>0.13369</v>
       </c>
       <c r="F52" t="n">
-        <v>0.11358</v>
+        <v>14.16246</v>
       </c>
       <c r="G52" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H52" t="n">
         <v>10</v>
@@ -1809,19 +1809,19 @@
         <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0054</v>
+        <v>0.49659</v>
       </c>
       <c r="E53" t="n">
-        <v>0.00135</v>
+        <v>0.12415</v>
       </c>
       <c r="F53" t="n">
-        <v>0.20916</v>
+        <v>19.38514</v>
       </c>
       <c r="G53" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H53" t="n">
         <v>11</v>
@@ -1835,19 +1835,19 @@
         <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D54" t="n">
-        <v>0.00445</v>
+        <v>0.5460700000000001</v>
       </c>
       <c r="E54" t="n">
-        <v>0.00111</v>
+        <v>0.13652</v>
       </c>
       <c r="F54" t="n">
-        <v>0.11613</v>
+        <v>15.08071</v>
       </c>
       <c r="G54" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H54" t="n">
         <v>12</v>
@@ -1861,19 +1861,19 @@
         <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D55" t="n">
-        <v>0.00505</v>
+        <v>0.95025</v>
       </c>
       <c r="E55" t="n">
-        <v>0.00126</v>
+        <v>0.23756</v>
       </c>
       <c r="F55" t="n">
-        <v>0.16749</v>
+        <v>21.27509</v>
       </c>
       <c r="G55" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H55" t="n">
         <v>13</v>
@@ -1887,19 +1887,19 @@
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D56" t="n">
-        <v>0.00627</v>
+        <v>0.71258</v>
       </c>
       <c r="E56" t="n">
-        <v>0.00157</v>
+        <v>0.17815</v>
       </c>
       <c r="F56" t="n">
-        <v>0.17325</v>
+        <v>13.95418</v>
       </c>
       <c r="G56" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H56" t="n">
         <v>14</v>
@@ -1913,19 +1913,19 @@
         <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0069</v>
+        <v>0.52032</v>
       </c>
       <c r="E57" t="n">
-        <v>0.00173</v>
+        <v>0.13008</v>
       </c>
       <c r="F57" t="n">
-        <v>0.20624</v>
+        <v>16.45964</v>
       </c>
       <c r="G57" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H57" t="n">
         <v>15</v>
@@ -1939,19 +1939,19 @@
         <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D58" t="n">
-        <v>0.00784</v>
+        <v>0.41565</v>
       </c>
       <c r="E58" t="n">
-        <v>0.00196</v>
+        <v>0.10391</v>
       </c>
       <c r="F58" t="n">
-        <v>0.26464</v>
+        <v>8.2462</v>
       </c>
       <c r="G58" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H58" t="n">
         <v>16</v>
@@ -1965,19 +1965,19 @@
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00576</v>
+        <v>0.91979</v>
       </c>
       <c r="E59" t="n">
-        <v>0.00144</v>
+        <v>0.22995</v>
       </c>
       <c r="F59" t="n">
-        <v>0.19516</v>
+        <v>18.01875</v>
       </c>
       <c r="G59" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H59" t="n">
         <v>17</v>
@@ -1991,19 +1991,19 @@
         <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D60" t="n">
-        <v>0.008750000000000001</v>
+        <v>0.6223</v>
       </c>
       <c r="E60" t="n">
-        <v>0.00219</v>
+        <v>0.15558</v>
       </c>
       <c r="F60" t="n">
-        <v>0.27323</v>
+        <v>14.1997</v>
       </c>
       <c r="G60" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H60" t="n">
         <v>18</v>
@@ -2017,19 +2017,19 @@
         <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D61" t="n">
-        <v>0.00683</v>
+        <v>0.77747</v>
       </c>
       <c r="E61" t="n">
-        <v>0.00171</v>
+        <v>0.19437</v>
       </c>
       <c r="F61" t="n">
-        <v>0.21475</v>
+        <v>18.84535</v>
       </c>
       <c r="G61" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H61" t="n">
         <v>19</v>
@@ -2043,19 +2043,19 @@
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D62" t="n">
-        <v>0.01039</v>
+        <v>0.38991</v>
       </c>
       <c r="E62" t="n">
-        <v>0.0026</v>
+        <v>0.09748</v>
       </c>
       <c r="F62" t="n">
-        <v>0.21081</v>
+        <v>10.30268</v>
       </c>
       <c r="G62" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2069,19 +2069,19 @@
         <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D63" t="n">
-        <v>0.00517</v>
+        <v>0.40692</v>
       </c>
       <c r="E63" t="n">
-        <v>0.00129</v>
+        <v>0.10173</v>
       </c>
       <c r="F63" t="n">
-        <v>0.10221</v>
+        <v>11.7787</v>
       </c>
       <c r="G63" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H63" t="n">
         <v>1</v>
@@ -2095,19 +2095,19 @@
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D64" t="n">
-        <v>0.00466</v>
+        <v>0.33278</v>
       </c>
       <c r="E64" t="n">
-        <v>0.00116</v>
+        <v>0.0832</v>
       </c>
       <c r="F64" t="n">
-        <v>0.09150999999999999</v>
+        <v>11.59768</v>
       </c>
       <c r="G64" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H64" t="n">
         <v>2</v>
@@ -2121,19 +2121,19 @@
         <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D65" t="n">
-        <v>0.00547</v>
+        <v>0.63136</v>
       </c>
       <c r="E65" t="n">
-        <v>0.00137</v>
+        <v>0.15784</v>
       </c>
       <c r="F65" t="n">
-        <v>0.09251</v>
+        <v>17.2393</v>
       </c>
       <c r="G65" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H65" t="n">
         <v>3</v>
@@ -2147,19 +2147,19 @@
         <v>1</v>
       </c>
       <c r="C66" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00958</v>
+        <v>0.36326</v>
       </c>
       <c r="E66" t="n">
-        <v>0.0024</v>
+        <v>0.09081</v>
       </c>
       <c r="F66" t="n">
-        <v>0.26173</v>
+        <v>14.23685</v>
       </c>
       <c r="G66" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H66" t="n">
         <v>4</v>
@@ -2173,19 +2173,19 @@
         <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D67" t="n">
-        <v>0.00697</v>
+        <v>0.52168</v>
       </c>
       <c r="E67" t="n">
-        <v>0.00174</v>
+        <v>0.13042</v>
       </c>
       <c r="F67" t="n">
-        <v>0.12358</v>
+        <v>13.83716</v>
       </c>
       <c r="G67" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H67" t="n">
         <v>5</v>
@@ -2199,19 +2199,19 @@
         <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D68" t="n">
-        <v>0.00721</v>
+        <v>0.14976</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0018</v>
+        <v>0.03744</v>
       </c>
       <c r="F68" t="n">
-        <v>0.18333</v>
+        <v>6.36846</v>
       </c>
       <c r="G68" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H68" t="n">
         <v>6</v>
@@ -2225,19 +2225,19 @@
         <v>1</v>
       </c>
       <c r="C69" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D69" t="n">
-        <v>0.00712</v>
+        <v>0.19087</v>
       </c>
       <c r="E69" t="n">
-        <v>0.00178</v>
+        <v>0.04772</v>
       </c>
       <c r="F69" t="n">
-        <v>0.10562</v>
+        <v>7.24823</v>
       </c>
       <c r="G69" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H69" t="n">
         <v>7</v>
@@ -2251,19 +2251,19 @@
         <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00726</v>
+        <v>0.16689</v>
       </c>
       <c r="E70" t="n">
-        <v>0.00181</v>
+        <v>0.04172</v>
       </c>
       <c r="F70" t="n">
-        <v>0.10659</v>
+        <v>7.06287</v>
       </c>
       <c r="G70" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H70" t="n">
         <v>8</v>
@@ -2277,19 +2277,19 @@
         <v>1</v>
       </c>
       <c r="C71" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00674</v>
+        <v>0.24969</v>
       </c>
       <c r="E71" t="n">
-        <v>0.00169</v>
+        <v>0.06242</v>
       </c>
       <c r="F71" t="n">
-        <v>0.14459</v>
+        <v>9.338939999999999</v>
       </c>
       <c r="G71" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H71" t="n">
         <v>9</v>
@@ -2303,19 +2303,19 @@
         <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D72" t="n">
-        <v>0.01035</v>
+        <v>0.3724</v>
       </c>
       <c r="E72" t="n">
-        <v>0.00259</v>
+        <v>0.0931</v>
       </c>
       <c r="F72" t="n">
-        <v>0.17903</v>
+        <v>9.7166</v>
       </c>
       <c r="G72" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H72" t="n">
         <v>10</v>
@@ -2329,19 +2329,19 @@
         <v>1</v>
       </c>
       <c r="C73" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D73" t="n">
-        <v>0.00639</v>
+        <v>0.25464</v>
       </c>
       <c r="E73" t="n">
-        <v>0.0016</v>
+        <v>0.06365999999999999</v>
       </c>
       <c r="F73" t="n">
-        <v>0.13816</v>
+        <v>7.38235</v>
       </c>
       <c r="G73" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H73" t="n">
         <v>11</v>
@@ -2355,19 +2355,19 @@
         <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D74" t="n">
-        <v>0.00992</v>
+        <v>0.33661</v>
       </c>
       <c r="E74" t="n">
-        <v>0.00248</v>
+        <v>0.08415</v>
       </c>
       <c r="F74" t="n">
-        <v>0.23112</v>
+        <v>7.9909</v>
       </c>
       <c r="G74" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H74" t="n">
         <v>12</v>
@@ -2381,19 +2381,19 @@
         <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00692</v>
+        <v>0.28229</v>
       </c>
       <c r="E75" t="n">
-        <v>0.00173</v>
+        <v>0.07056999999999999</v>
       </c>
       <c r="F75" t="n">
-        <v>0.1424</v>
+        <v>9.85412</v>
       </c>
       <c r="G75" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H75" t="n">
         <v>13</v>
@@ -2407,19 +2407,19 @@
         <v>1</v>
       </c>
       <c r="C76" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00727</v>
+        <v>0.3685</v>
       </c>
       <c r="E76" t="n">
-        <v>0.00182</v>
+        <v>0.09211999999999999</v>
       </c>
       <c r="F76" t="n">
-        <v>0.12658</v>
+        <v>8.413309999999999</v>
       </c>
       <c r="G76" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H76" t="n">
         <v>14</v>
@@ -2433,19 +2433,19 @@
         <v>1</v>
       </c>
       <c r="C77" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D77" t="n">
-        <v>0.00687</v>
+        <v>0.32816</v>
       </c>
       <c r="E77" t="n">
-        <v>0.00172</v>
+        <v>0.08204</v>
       </c>
       <c r="F77" t="n">
-        <v>0.17516</v>
+        <v>10.15683</v>
       </c>
       <c r="G77" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H77" t="n">
         <v>15</v>
@@ -2459,19 +2459,19 @@
         <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00725</v>
+        <v>0.32987</v>
       </c>
       <c r="E78" t="n">
-        <v>0.00181</v>
+        <v>0.08247</v>
       </c>
       <c r="F78" t="n">
-        <v>0.12724</v>
+        <v>9.680709999999999</v>
       </c>
       <c r="G78" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H78" t="n">
         <v>16</v>
@@ -2485,19 +2485,19 @@
         <v>1</v>
       </c>
       <c r="C79" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D79" t="n">
-        <v>0.00608</v>
+        <v>0.29543</v>
       </c>
       <c r="E79" t="n">
-        <v>0.00152</v>
+        <v>0.07386</v>
       </c>
       <c r="F79" t="n">
-        <v>0.12657</v>
+        <v>7.9829</v>
       </c>
       <c r="G79" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H79" t="n">
         <v>17</v>
@@ -2511,19 +2511,19 @@
         <v>1</v>
       </c>
       <c r="C80" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D80" t="n">
-        <v>0.0062</v>
+        <v>0.23228</v>
       </c>
       <c r="E80" t="n">
-        <v>0.00155</v>
+        <v>0.05807</v>
       </c>
       <c r="F80" t="n">
-        <v>0.13514</v>
+        <v>6.42128</v>
       </c>
       <c r="G80" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H80" t="n">
         <v>18</v>
@@ -2540,16 +2540,16 @@
         <v>23</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00774</v>
+        <v>0.20288</v>
       </c>
       <c r="E81" t="n">
-        <v>0.00193</v>
+        <v>0.05072</v>
       </c>
       <c r="F81" t="n">
-        <v>0.18295</v>
+        <v>5.89931</v>
       </c>
       <c r="G81" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H81" t="n">
         <v>19</v>
@@ -2563,16 +2563,16 @@
         <v>1</v>
       </c>
       <c r="C82" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D82" t="n">
-        <v>0.00751</v>
+        <v>0.36458</v>
       </c>
       <c r="E82" t="n">
-        <v>0.00125</v>
+        <v>0.06076</v>
       </c>
       <c r="F82" t="n">
-        <v>0.17781</v>
+        <v>7.37494</v>
       </c>
       <c r="G82" t="n">
         <v>0.85</v>
@@ -2589,16 +2589,16 @@
         <v>1</v>
       </c>
       <c r="C83" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D83" t="n">
-        <v>0.009889999999999999</v>
+        <v>0.51594</v>
       </c>
       <c r="E83" t="n">
-        <v>0.00165</v>
+        <v>0.08599</v>
       </c>
       <c r="F83" t="n">
-        <v>0.27292</v>
+        <v>13.52079</v>
       </c>
       <c r="G83" t="n">
         <v>0.85</v>
@@ -2615,16 +2615,16 @@
         <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D84" t="n">
-        <v>0.00727</v>
+        <v>0.56098</v>
       </c>
       <c r="E84" t="n">
-        <v>0.00121</v>
+        <v>0.0935</v>
       </c>
       <c r="F84" t="n">
-        <v>0.26111</v>
+        <v>13.17485</v>
       </c>
       <c r="G84" t="n">
         <v>0.85</v>
@@ -2641,16 +2641,16 @@
         <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D85" t="n">
-        <v>0.01143</v>
+        <v>0.40782</v>
       </c>
       <c r="E85" t="n">
-        <v>0.00191</v>
+        <v>0.06797</v>
       </c>
       <c r="F85" t="n">
-        <v>0.24412</v>
+        <v>9.39179</v>
       </c>
       <c r="G85" t="n">
         <v>0.85</v>
@@ -2667,16 +2667,16 @@
         <v>1</v>
       </c>
       <c r="C86" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D86" t="n">
-        <v>0.00768</v>
+        <v>0.43316</v>
       </c>
       <c r="E86" t="n">
-        <v>0.00128</v>
+        <v>0.07219</v>
       </c>
       <c r="F86" t="n">
-        <v>0.13556</v>
+        <v>10.51531</v>
       </c>
       <c r="G86" t="n">
         <v>0.85</v>
@@ -2693,16 +2693,16 @@
         <v>1</v>
       </c>
       <c r="C87" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D87" t="n">
-        <v>0.00826</v>
+        <v>0.48938</v>
       </c>
       <c r="E87" t="n">
-        <v>0.00138</v>
+        <v>0.08155999999999999</v>
       </c>
       <c r="F87" t="n">
-        <v>0.11339</v>
+        <v>14.59051</v>
       </c>
       <c r="G87" t="n">
         <v>0.85</v>
@@ -2719,16 +2719,16 @@
         <v>1</v>
       </c>
       <c r="C88" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D88" t="n">
-        <v>0.00812</v>
+        <v>0.3027</v>
       </c>
       <c r="E88" t="n">
-        <v>0.00135</v>
+        <v>0.05045</v>
       </c>
       <c r="F88" t="n">
-        <v>0.18162</v>
+        <v>6.69441</v>
       </c>
       <c r="G88" t="n">
         <v>0.85</v>
@@ -2745,16 +2745,16 @@
         <v>1</v>
       </c>
       <c r="C89" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D89" t="n">
-        <v>0.008840000000000001</v>
+        <v>0.38287</v>
       </c>
       <c r="E89" t="n">
-        <v>0.00147</v>
+        <v>0.06381000000000001</v>
       </c>
       <c r="F89" t="n">
-        <v>0.16706</v>
+        <v>9.641260000000001</v>
       </c>
       <c r="G89" t="n">
         <v>0.85</v>
@@ -2771,16 +2771,16 @@
         <v>1</v>
       </c>
       <c r="C90" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D90" t="n">
-        <v>0.008869999999999999</v>
+        <v>0.5305299999999999</v>
       </c>
       <c r="E90" t="n">
-        <v>0.00148</v>
+        <v>0.08842</v>
       </c>
       <c r="F90" t="n">
-        <v>0.17356</v>
+        <v>10.31262</v>
       </c>
       <c r="G90" t="n">
         <v>0.85</v>
@@ -2797,16 +2797,16 @@
         <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D91" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.3137</v>
       </c>
       <c r="E91" t="n">
-        <v>0.00147</v>
+        <v>0.05228</v>
       </c>
       <c r="F91" t="n">
-        <v>0.16365</v>
+        <v>7.13235</v>
       </c>
       <c r="G91" t="n">
         <v>0.85</v>
@@ -2823,16 +2823,16 @@
         <v>1</v>
       </c>
       <c r="C92" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D92" t="n">
-        <v>0.00827</v>
+        <v>0.22491</v>
       </c>
       <c r="E92" t="n">
-        <v>0.00138</v>
+        <v>0.03748</v>
       </c>
       <c r="F92" t="n">
-        <v>0.14761</v>
+        <v>6.88781</v>
       </c>
       <c r="G92" t="n">
         <v>0.85</v>
@@ -2849,16 +2849,16 @@
         <v>1</v>
       </c>
       <c r="C93" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00603</v>
+        <v>0.29333</v>
       </c>
       <c r="E93" t="n">
-        <v>0.001</v>
+        <v>0.04889</v>
       </c>
       <c r="F93" t="n">
-        <v>0.11852</v>
+        <v>8.75037</v>
       </c>
       <c r="G93" t="n">
         <v>0.85</v>
@@ -2875,16 +2875,16 @@
         <v>1</v>
       </c>
       <c r="C94" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D94" t="n">
-        <v>0.02463</v>
+        <v>0.49216</v>
       </c>
       <c r="E94" t="n">
-        <v>0.0041</v>
+        <v>0.08203000000000001</v>
       </c>
       <c r="F94" t="n">
-        <v>0.67598</v>
+        <v>12.96611</v>
       </c>
       <c r="G94" t="n">
         <v>0.85</v>
@@ -2901,16 +2901,16 @@
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D95" t="n">
-        <v>0.00731</v>
+        <v>0.45163</v>
       </c>
       <c r="E95" t="n">
-        <v>0.00122</v>
+        <v>0.07527</v>
       </c>
       <c r="F95" t="n">
-        <v>0.13558</v>
+        <v>11.24921</v>
       </c>
       <c r="G95" t="n">
         <v>0.85</v>
@@ -2927,16 +2927,16 @@
         <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0074</v>
+        <v>0.2905</v>
       </c>
       <c r="E96" t="n">
-        <v>0.00123</v>
+        <v>0.04842</v>
       </c>
       <c r="F96" t="n">
-        <v>0.10704</v>
+        <v>10.06408</v>
       </c>
       <c r="G96" t="n">
         <v>0.85</v>
@@ -2953,16 +2953,16 @@
         <v>1</v>
       </c>
       <c r="C97" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D97" t="n">
-        <v>0.00566</v>
+        <v>0.52059</v>
       </c>
       <c r="E97" t="n">
-        <v>0.00094</v>
+        <v>0.08676</v>
       </c>
       <c r="F97" t="n">
-        <v>0.06158</v>
+        <v>9.408569999999999</v>
       </c>
       <c r="G97" t="n">
         <v>0.85</v>
@@ -2979,16 +2979,16 @@
         <v>1</v>
       </c>
       <c r="C98" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D98" t="n">
-        <v>0.008959999999999999</v>
+        <v>0.50285</v>
       </c>
       <c r="E98" t="n">
-        <v>0.00149</v>
+        <v>0.08381</v>
       </c>
       <c r="F98" t="n">
-        <v>0.10452</v>
+        <v>12.23539</v>
       </c>
       <c r="G98" t="n">
         <v>0.85</v>
@@ -3005,16 +3005,16 @@
         <v>1</v>
       </c>
       <c r="C99" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D99" t="n">
-        <v>0.00915</v>
+        <v>0.30019</v>
       </c>
       <c r="E99" t="n">
-        <v>0.00152</v>
+        <v>0.05003</v>
       </c>
       <c r="F99" t="n">
-        <v>0.17066</v>
+        <v>7.87812</v>
       </c>
       <c r="G99" t="n">
         <v>0.85</v>
@@ -3031,16 +3031,16 @@
         <v>1</v>
       </c>
       <c r="C100" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D100" t="n">
-        <v>0.0083</v>
+        <v>0.82938</v>
       </c>
       <c r="E100" t="n">
-        <v>0.00138</v>
+        <v>0.13823</v>
       </c>
       <c r="F100" t="n">
-        <v>0.14613</v>
+        <v>17.32949</v>
       </c>
       <c r="G100" t="n">
         <v>0.85</v>
@@ -3057,16 +3057,16 @@
         <v>1</v>
       </c>
       <c r="C101" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D101" t="n">
-        <v>0.009299999999999999</v>
+        <v>0.44613</v>
       </c>
       <c r="E101" t="n">
-        <v>0.00155</v>
+        <v>0.07436</v>
       </c>
       <c r="F101" t="n">
-        <v>0.16402</v>
+        <v>10.101</v>
       </c>
       <c r="G101" t="n">
         <v>0.85</v>
@@ -3083,16 +3083,16 @@
         <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D102" t="n">
-        <v>0.01133</v>
+        <v>1.00537</v>
       </c>
       <c r="E102" t="n">
-        <v>0.00189</v>
+        <v>0.16756</v>
       </c>
       <c r="F102" t="n">
-        <v>0.16367</v>
+        <v>18.22265</v>
       </c>
       <c r="G102" t="n">
         <v>0.15</v>
@@ -3109,16 +3109,16 @@
         <v>1</v>
       </c>
       <c r="C103" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D103" t="n">
-        <v>0.00894</v>
+        <v>0.32444</v>
       </c>
       <c r="E103" t="n">
-        <v>0.00149</v>
+        <v>0.05407</v>
       </c>
       <c r="F103" t="n">
-        <v>0.06559</v>
+        <v>6.83268</v>
       </c>
       <c r="G103" t="n">
         <v>0.15</v>
@@ -3135,16 +3135,16 @@
         <v>1</v>
       </c>
       <c r="C104" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D104" t="n">
-        <v>0.00712</v>
+        <v>0.43982</v>
       </c>
       <c r="E104" t="n">
-        <v>0.00119</v>
+        <v>0.0733</v>
       </c>
       <c r="F104" t="n">
-        <v>0.09562</v>
+        <v>8.36482</v>
       </c>
       <c r="G104" t="n">
         <v>0.15</v>
@@ -3161,16 +3161,16 @@
         <v>1</v>
       </c>
       <c r="C105" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D105" t="n">
-        <v>0.01381</v>
+        <v>0.71475</v>
       </c>
       <c r="E105" t="n">
-        <v>0.0023</v>
+        <v>0.11912</v>
       </c>
       <c r="F105" t="n">
-        <v>0.18652</v>
+        <v>12.52712</v>
       </c>
       <c r="G105" t="n">
         <v>0.15</v>
@@ -3187,16 +3187,16 @@
         <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D106" t="n">
-        <v>0.01147</v>
+        <v>0.56226</v>
       </c>
       <c r="E106" t="n">
-        <v>0.00191</v>
+        <v>0.09371</v>
       </c>
       <c r="F106" t="n">
-        <v>0.14363</v>
+        <v>8.855079999999999</v>
       </c>
       <c r="G106" t="n">
         <v>0.15</v>
@@ -3213,16 +3213,16 @@
         <v>1</v>
       </c>
       <c r="C107" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D107" t="n">
-        <v>0.01122</v>
+        <v>0.29685</v>
       </c>
       <c r="E107" t="n">
-        <v>0.00187</v>
+        <v>0.04948</v>
       </c>
       <c r="F107" t="n">
-        <v>0.16403</v>
+        <v>7.02361</v>
       </c>
       <c r="G107" t="n">
         <v>0.15</v>
@@ -3239,16 +3239,16 @@
         <v>1</v>
       </c>
       <c r="C108" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D108" t="n">
-        <v>0.01151</v>
+        <v>1.04515</v>
       </c>
       <c r="E108" t="n">
-        <v>0.00192</v>
+        <v>0.17419</v>
       </c>
       <c r="F108" t="n">
-        <v>0.19975</v>
+        <v>18.00204</v>
       </c>
       <c r="G108" t="n">
         <v>0.15</v>
@@ -3265,16 +3265,16 @@
         <v>1</v>
       </c>
       <c r="C109" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D109" t="n">
-        <v>0.01609</v>
+        <v>0.61029</v>
       </c>
       <c r="E109" t="n">
-        <v>0.00268</v>
+        <v>0.10172</v>
       </c>
       <c r="F109" t="n">
-        <v>0.21316</v>
+        <v>7.71621</v>
       </c>
       <c r="G109" t="n">
         <v>0.15</v>
@@ -3291,16 +3291,16 @@
         <v>1</v>
       </c>
       <c r="C110" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D110" t="n">
-        <v>0.01433</v>
+        <v>0.81048</v>
       </c>
       <c r="E110" t="n">
-        <v>0.00239</v>
+        <v>0.13508</v>
       </c>
       <c r="F110" t="n">
-        <v>0.162</v>
+        <v>16.66201</v>
       </c>
       <c r="G110" t="n">
         <v>0.15</v>
@@ -3317,16 +3317,16 @@
         <v>1</v>
       </c>
       <c r="C111" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D111" t="n">
-        <v>0.009639999999999999</v>
+        <v>0.71275</v>
       </c>
       <c r="E111" t="n">
-        <v>0.00161</v>
+        <v>0.11879</v>
       </c>
       <c r="F111" t="n">
-        <v>0.14964</v>
+        <v>10.90441</v>
       </c>
       <c r="G111" t="n">
         <v>0.15</v>
@@ -3343,16 +3343,16 @@
         <v>1</v>
       </c>
       <c r="C112" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D112" t="n">
-        <v>0.00822</v>
+        <v>0.57838</v>
       </c>
       <c r="E112" t="n">
-        <v>0.00137</v>
+        <v>0.0964</v>
       </c>
       <c r="F112" t="n">
-        <v>0.13551</v>
+        <v>12.7074</v>
       </c>
       <c r="G112" t="n">
         <v>0.15</v>
@@ -3369,16 +3369,16 @@
         <v>1</v>
       </c>
       <c r="C113" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D113" t="n">
-        <v>0.00852</v>
+        <v>0.86817</v>
       </c>
       <c r="E113" t="n">
-        <v>0.00142</v>
+        <v>0.1447</v>
       </c>
       <c r="F113" t="n">
-        <v>0.142</v>
+        <v>11.20058</v>
       </c>
       <c r="G113" t="n">
         <v>0.15</v>
@@ -3395,16 +3395,16 @@
         <v>1</v>
       </c>
       <c r="C114" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D114" t="n">
-        <v>0.00736</v>
+        <v>0.50856</v>
       </c>
       <c r="E114" t="n">
-        <v>0.00123</v>
+        <v>0.08476</v>
       </c>
       <c r="F114" t="n">
-        <v>0.05663</v>
+        <v>10.80618</v>
       </c>
       <c r="G114" t="n">
         <v>0.15</v>
@@ -3421,16 +3421,16 @@
         <v>1</v>
       </c>
       <c r="C115" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D115" t="n">
-        <v>0.0114</v>
+        <v>0.72927</v>
       </c>
       <c r="E115" t="n">
-        <v>0.0019</v>
+        <v>0.12155</v>
       </c>
       <c r="F115" t="n">
-        <v>0.15322</v>
+        <v>12.0554</v>
       </c>
       <c r="G115" t="n">
         <v>0.15</v>
@@ -3447,16 +3447,16 @@
         <v>1</v>
       </c>
       <c r="C116" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D116" t="n">
-        <v>0.01837</v>
+        <v>0.48484</v>
       </c>
       <c r="E116" t="n">
-        <v>0.00306</v>
+        <v>0.08081000000000001</v>
       </c>
       <c r="F116" t="n">
-        <v>0.20803</v>
+        <v>13.12043</v>
       </c>
       <c r="G116" t="n">
         <v>0.15</v>
@@ -3473,16 +3473,16 @@
         <v>1</v>
       </c>
       <c r="C117" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D117" t="n">
-        <v>0.0129</v>
+        <v>0.48425</v>
       </c>
       <c r="E117" t="n">
-        <v>0.00215</v>
+        <v>0.08071</v>
       </c>
       <c r="F117" t="n">
-        <v>0.1608</v>
+        <v>7.1008</v>
       </c>
       <c r="G117" t="n">
         <v>0.15</v>
@@ -3502,13 +3502,13 @@
         <v>12</v>
       </c>
       <c r="D118" t="n">
-        <v>0.01108</v>
+        <v>0.59875</v>
       </c>
       <c r="E118" t="n">
-        <v>0.00185</v>
+        <v>0.09979</v>
       </c>
       <c r="F118" t="n">
-        <v>0.13798</v>
+        <v>9.231070000000001</v>
       </c>
       <c r="G118" t="n">
         <v>0.15</v>
@@ -3525,16 +3525,16 @@
         <v>1</v>
       </c>
       <c r="C119" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D119" t="n">
-        <v>0.01623</v>
+        <v>0.49148</v>
       </c>
       <c r="E119" t="n">
-        <v>0.00271</v>
+        <v>0.08191</v>
       </c>
       <c r="F119" t="n">
-        <v>0.26369</v>
+        <v>7.05475</v>
       </c>
       <c r="G119" t="n">
         <v>0.15</v>
@@ -3551,16 +3551,16 @@
         <v>1</v>
       </c>
       <c r="C120" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D120" t="n">
-        <v>0.01409</v>
+        <v>0.28068</v>
       </c>
       <c r="E120" t="n">
-        <v>0.00235</v>
+        <v>0.04678</v>
       </c>
       <c r="F120" t="n">
-        <v>0.17503</v>
+        <v>4.01767</v>
       </c>
       <c r="G120" t="n">
         <v>0.15</v>
@@ -3577,16 +3577,16 @@
         <v>1</v>
       </c>
       <c r="C121" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D121" t="n">
-        <v>0.01081</v>
+        <v>0.31838</v>
       </c>
       <c r="E121" t="n">
-        <v>0.0018</v>
+        <v>0.05306</v>
       </c>
       <c r="F121" t="n">
-        <v>0.1691</v>
+        <v>7.64663</v>
       </c>
       <c r="G121" t="n">
         <v>0.15</v>
@@ -3603,19 +3603,19 @@
         <v>1</v>
       </c>
       <c r="C122" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D122" t="n">
-        <v>0.01291</v>
+        <v>0.46871</v>
       </c>
       <c r="E122" t="n">
-        <v>0.00161</v>
+        <v>0.05859</v>
       </c>
       <c r="F122" t="n">
-        <v>0.18575</v>
+        <v>6.50146</v>
       </c>
       <c r="G122" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H122" t="n">
         <v>0</v>
@@ -3629,19 +3629,19 @@
         <v>1</v>
       </c>
       <c r="C123" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D123" t="n">
-        <v>0.01211</v>
+        <v>0.49914</v>
       </c>
       <c r="E123" t="n">
-        <v>0.00151</v>
+        <v>0.06239</v>
       </c>
       <c r="F123" t="n">
-        <v>0.29662</v>
+        <v>6.68596</v>
       </c>
       <c r="G123" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H123" t="n">
         <v>1</v>
@@ -3655,19 +3655,19 @@
         <v>1</v>
       </c>
       <c r="C124" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D124" t="n">
-        <v>0.0102</v>
+        <v>0.85328</v>
       </c>
       <c r="E124" t="n">
-        <v>0.00128</v>
+        <v>0.10666</v>
       </c>
       <c r="F124" t="n">
-        <v>0.16826</v>
+        <v>14.39901</v>
       </c>
       <c r="G124" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H124" t="n">
         <v>2</v>
@@ -3681,19 +3681,19 @@
         <v>1</v>
       </c>
       <c r="C125" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D125" t="n">
-        <v>0.01956</v>
+        <v>0.73082</v>
       </c>
       <c r="E125" t="n">
-        <v>0.00245</v>
+        <v>0.09135</v>
       </c>
       <c r="F125" t="n">
-        <v>0.26029</v>
+        <v>10.37944</v>
       </c>
       <c r="G125" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H125" t="n">
         <v>3</v>
@@ -3707,19 +3707,19 @@
         <v>1</v>
       </c>
       <c r="C126" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D126" t="n">
-        <v>0.01226</v>
+        <v>0.73641</v>
       </c>
       <c r="E126" t="n">
-        <v>0.00153</v>
+        <v>0.09205000000000001</v>
       </c>
       <c r="F126" t="n">
-        <v>0.20014</v>
+        <v>9.494820000000001</v>
       </c>
       <c r="G126" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H126" t="n">
         <v>4</v>
@@ -3733,19 +3733,19 @@
         <v>1</v>
       </c>
       <c r="C127" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0161</v>
+        <v>0.65823</v>
       </c>
       <c r="E127" t="n">
-        <v>0.00201</v>
+        <v>0.08228000000000001</v>
       </c>
       <c r="F127" t="n">
-        <v>0.21933</v>
+        <v>10.48199</v>
       </c>
       <c r="G127" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H127" t="n">
         <v>5</v>
@@ -3759,19 +3759,19 @@
         <v>1</v>
       </c>
       <c r="C128" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D128" t="n">
-        <v>0.00933</v>
+        <v>0.4205</v>
       </c>
       <c r="E128" t="n">
-        <v>0.00117</v>
+        <v>0.05256</v>
       </c>
       <c r="F128" t="n">
-        <v>0.08066</v>
+        <v>5.60596</v>
       </c>
       <c r="G128" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H128" t="n">
         <v>6</v>
@@ -3785,19 +3785,19 @@
         <v>1</v>
       </c>
       <c r="C129" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D129" t="n">
-        <v>0.01206</v>
+        <v>0.5439000000000001</v>
       </c>
       <c r="E129" t="n">
-        <v>0.00151</v>
+        <v>0.06798999999999999</v>
       </c>
       <c r="F129" t="n">
-        <v>0.19796</v>
+        <v>9.69229</v>
       </c>
       <c r="G129" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H129" t="n">
         <v>7</v>
@@ -3811,19 +3811,19 @@
         <v>1</v>
       </c>
       <c r="C130" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D130" t="n">
-        <v>0.01296</v>
+        <v>0.63186</v>
       </c>
       <c r="E130" t="n">
-        <v>0.00162</v>
+        <v>0.07897999999999999</v>
       </c>
       <c r="F130" t="n">
-        <v>0.2302</v>
+        <v>9.96078</v>
       </c>
       <c r="G130" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H130" t="n">
         <v>8</v>
@@ -3837,19 +3837,19 @@
         <v>1</v>
       </c>
       <c r="C131" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D131" t="n">
-        <v>0.01691</v>
+        <v>0.83417</v>
       </c>
       <c r="E131" t="n">
-        <v>0.00211</v>
+        <v>0.10427</v>
       </c>
       <c r="F131" t="n">
-        <v>0.40589</v>
+        <v>10.5513</v>
       </c>
       <c r="G131" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H131" t="n">
         <v>9</v>
@@ -3863,19 +3863,19 @@
         <v>1</v>
       </c>
       <c r="C132" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D132" t="n">
-        <v>0.00912</v>
+        <v>0.67867</v>
       </c>
       <c r="E132" t="n">
-        <v>0.00114</v>
+        <v>0.08483</v>
       </c>
       <c r="F132" t="n">
-        <v>0.10531</v>
+        <v>7.91571</v>
       </c>
       <c r="G132" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H132" t="n">
         <v>10</v>
@@ -3889,19 +3889,19 @@
         <v>1</v>
       </c>
       <c r="C133" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D133" t="n">
-        <v>0.01544</v>
+        <v>0.50302</v>
       </c>
       <c r="E133" t="n">
-        <v>0.00193</v>
+        <v>0.06288000000000001</v>
       </c>
       <c r="F133" t="n">
-        <v>0.4878</v>
+        <v>7.77773</v>
       </c>
       <c r="G133" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H133" t="n">
         <v>11</v>
@@ -3915,19 +3915,19 @@
         <v>1</v>
       </c>
       <c r="C134" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D134" t="n">
-        <v>0.01118</v>
+        <v>0.60872</v>
       </c>
       <c r="E134" t="n">
-        <v>0.0014</v>
+        <v>0.07609</v>
       </c>
       <c r="F134" t="n">
-        <v>0.1626</v>
+        <v>9.802429999999999</v>
       </c>
       <c r="G134" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H134" t="n">
         <v>12</v>
@@ -3941,19 +3941,19 @@
         <v>1</v>
       </c>
       <c r="C135" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D135" t="n">
-        <v>0.0104</v>
+        <v>0.7779700000000001</v>
       </c>
       <c r="E135" t="n">
-        <v>0.0013</v>
+        <v>0.09725</v>
       </c>
       <c r="F135" t="n">
-        <v>0.18186</v>
+        <v>9.49039</v>
       </c>
       <c r="G135" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H135" t="n">
         <v>13</v>
@@ -3967,19 +3967,19 @@
         <v>1</v>
       </c>
       <c r="C136" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D136" t="n">
-        <v>0.00822</v>
+        <v>0.55675</v>
       </c>
       <c r="E136" t="n">
-        <v>0.00103</v>
+        <v>0.06959</v>
       </c>
       <c r="F136" t="n">
-        <v>0.10509</v>
+        <v>7.33305</v>
       </c>
       <c r="G136" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H136" t="n">
         <v>14</v>
@@ -3993,19 +3993,19 @@
         <v>1</v>
       </c>
       <c r="C137" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D137" t="n">
-        <v>0.01793</v>
+        <v>0.5342</v>
       </c>
       <c r="E137" t="n">
-        <v>0.00224</v>
+        <v>0.06677</v>
       </c>
       <c r="F137" t="n">
-        <v>0.23909</v>
+        <v>7.00479</v>
       </c>
       <c r="G137" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H137" t="n">
         <v>15</v>
@@ -4019,19 +4019,19 @@
         <v>1</v>
       </c>
       <c r="C138" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D138" t="n">
-        <v>0.00975</v>
+        <v>0.8027</v>
       </c>
       <c r="E138" t="n">
-        <v>0.00122</v>
+        <v>0.10034</v>
       </c>
       <c r="F138" t="n">
-        <v>0.10359</v>
+        <v>9.005979999999999</v>
       </c>
       <c r="G138" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H138" t="n">
         <v>16</v>
@@ -4045,19 +4045,19 @@
         <v>1</v>
       </c>
       <c r="C139" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D139" t="n">
-        <v>0.01104</v>
+        <v>0.93424</v>
       </c>
       <c r="E139" t="n">
-        <v>0.00138</v>
+        <v>0.11678</v>
       </c>
       <c r="F139" t="n">
-        <v>0.16148</v>
+        <v>17.50248</v>
       </c>
       <c r="G139" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H139" t="n">
         <v>17</v>
@@ -4071,19 +4071,19 @@
         <v>1</v>
       </c>
       <c r="C140" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D140" t="n">
-        <v>0.00877</v>
+        <v>0.69962</v>
       </c>
       <c r="E140" t="n">
-        <v>0.0011</v>
+        <v>0.08745</v>
       </c>
       <c r="F140" t="n">
-        <v>0.14529</v>
+        <v>13.9674</v>
       </c>
       <c r="G140" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H140" t="n">
         <v>18</v>
@@ -4097,19 +4097,19 @@
         <v>1</v>
       </c>
       <c r="C141" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D141" t="n">
-        <v>0.01738</v>
+        <v>0.55001</v>
       </c>
       <c r="E141" t="n">
-        <v>0.00217</v>
+        <v>0.06875000000000001</v>
       </c>
       <c r="F141" t="n">
-        <v>0.26669</v>
+        <v>4.30997</v>
       </c>
       <c r="G141" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
       <c r="H141" t="n">
         <v>19</v>
@@ -4123,19 +4123,19 @@
         <v>1</v>
       </c>
       <c r="C142" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D142" t="n">
-        <v>0.01596</v>
+        <v>0.7125899999999999</v>
       </c>
       <c r="E142" t="n">
-        <v>0.002</v>
+        <v>0.08907</v>
       </c>
       <c r="F142" t="n">
-        <v>0.16563</v>
+        <v>12.16579</v>
       </c>
       <c r="G142" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H142" t="n">
         <v>0</v>
@@ -4149,19 +4149,19 @@
         <v>1</v>
       </c>
       <c r="C143" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D143" t="n">
-        <v>0.01408</v>
+        <v>0.30158</v>
       </c>
       <c r="E143" t="n">
-        <v>0.00176</v>
+        <v>0.0377</v>
       </c>
       <c r="F143" t="n">
-        <v>0.10257</v>
+        <v>6.28605</v>
       </c>
       <c r="G143" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H143" t="n">
         <v>1</v>
@@ -4175,19 +4175,19 @@
         <v>1</v>
       </c>
       <c r="C144" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D144" t="n">
-        <v>0.01285</v>
+        <v>0.27817</v>
       </c>
       <c r="E144" t="n">
-        <v>0.00161</v>
+        <v>0.03477</v>
       </c>
       <c r="F144" t="n">
-        <v>0.16024</v>
+        <v>7.38957</v>
       </c>
       <c r="G144" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H144" t="n">
         <v>2</v>
@@ -4201,19 +4201,19 @@
         <v>1</v>
       </c>
       <c r="C145" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D145" t="n">
-        <v>0.0142</v>
+        <v>0.31954</v>
       </c>
       <c r="E145" t="n">
-        <v>0.00177</v>
+        <v>0.03994</v>
       </c>
       <c r="F145" t="n">
-        <v>0.11861</v>
+        <v>6.84593</v>
       </c>
       <c r="G145" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H145" t="n">
         <v>3</v>
@@ -4227,19 +4227,19 @@
         <v>1</v>
       </c>
       <c r="C146" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D146" t="n">
-        <v>0.01755</v>
+        <v>0.69307</v>
       </c>
       <c r="E146" t="n">
-        <v>0.00219</v>
+        <v>0.08663</v>
       </c>
       <c r="F146" t="n">
-        <v>0.19903</v>
+        <v>10.95939</v>
       </c>
       <c r="G146" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H146" t="n">
         <v>4</v>
@@ -4253,19 +4253,19 @@
         <v>1</v>
       </c>
       <c r="C147" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D147" t="n">
-        <v>0.01268</v>
+        <v>0.24077</v>
       </c>
       <c r="E147" t="n">
-        <v>0.00158</v>
+        <v>0.0301</v>
       </c>
       <c r="F147" t="n">
-        <v>0.15912</v>
+        <v>5.08969</v>
       </c>
       <c r="G147" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H147" t="n">
         <v>5</v>
@@ -4279,19 +4279,19 @@
         <v>1</v>
       </c>
       <c r="C148" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D148" t="n">
-        <v>0.01669</v>
+        <v>0.56236</v>
       </c>
       <c r="E148" t="n">
-        <v>0.00209</v>
+        <v>0.07029000000000001</v>
       </c>
       <c r="F148" t="n">
-        <v>0.19184</v>
+        <v>12.20239</v>
       </c>
       <c r="G148" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H148" t="n">
         <v>6</v>
@@ -4305,19 +4305,19 @@
         <v>1</v>
       </c>
       <c r="C149" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D149" t="n">
-        <v>0.00944</v>
+        <v>0.39072</v>
       </c>
       <c r="E149" t="n">
-        <v>0.00118</v>
+        <v>0.04884</v>
       </c>
       <c r="F149" t="n">
-        <v>0.07209</v>
+        <v>9.34782</v>
       </c>
       <c r="G149" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H149" t="n">
         <v>7</v>
@@ -4331,19 +4331,19 @@
         <v>1</v>
       </c>
       <c r="C150" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D150" t="n">
-        <v>0.01232</v>
+        <v>0.41506</v>
       </c>
       <c r="E150" t="n">
-        <v>0.00154</v>
+        <v>0.05188</v>
       </c>
       <c r="F150" t="n">
-        <v>0.12716</v>
+        <v>8.75901</v>
       </c>
       <c r="G150" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H150" t="n">
         <v>8</v>
@@ -4357,19 +4357,19 @@
         <v>1</v>
       </c>
       <c r="C151" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D151" t="n">
-        <v>0.02006</v>
+        <v>0.37152</v>
       </c>
       <c r="E151" t="n">
-        <v>0.00251</v>
+        <v>0.04644</v>
       </c>
       <c r="F151" t="n">
-        <v>0.2467</v>
+        <v>8.01422</v>
       </c>
       <c r="G151" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H151" t="n">
         <v>9</v>
@@ -4383,19 +4383,19 @@
         <v>1</v>
       </c>
       <c r="C152" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D152" t="n">
-        <v>0.00991</v>
+        <v>0.58072</v>
       </c>
       <c r="E152" t="n">
-        <v>0.00124</v>
+        <v>0.07259</v>
       </c>
       <c r="F152" t="n">
-        <v>0.05657</v>
+        <v>7.72003</v>
       </c>
       <c r="G152" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H152" t="n">
         <v>10</v>
@@ -4409,19 +4409,19 @@
         <v>1</v>
       </c>
       <c r="C153" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D153" t="n">
-        <v>0.01855</v>
+        <v>0.40601</v>
       </c>
       <c r="E153" t="n">
-        <v>0.00232</v>
+        <v>0.05075</v>
       </c>
       <c r="F153" t="n">
-        <v>0.19152</v>
+        <v>8.96256</v>
       </c>
       <c r="G153" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H153" t="n">
         <v>11</v>
@@ -4435,19 +4435,19 @@
         <v>1</v>
       </c>
       <c r="C154" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D154" t="n">
-        <v>0.01221</v>
+        <v>0.37699</v>
       </c>
       <c r="E154" t="n">
-        <v>0.00153</v>
+        <v>0.04712</v>
       </c>
       <c r="F154" t="n">
-        <v>0.07926999999999999</v>
+        <v>9.551310000000001</v>
       </c>
       <c r="G154" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H154" t="n">
         <v>12</v>
@@ -4461,19 +4461,19 @@
         <v>1</v>
       </c>
       <c r="C155" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D155" t="n">
-        <v>0.01657</v>
+        <v>0.39498</v>
       </c>
       <c r="E155" t="n">
-        <v>0.00207</v>
+        <v>0.04937</v>
       </c>
       <c r="F155" t="n">
-        <v>0.17066</v>
+        <v>10.69621</v>
       </c>
       <c r="G155" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H155" t="n">
         <v>13</v>
@@ -4487,19 +4487,19 @@
         <v>1</v>
       </c>
       <c r="C156" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D156" t="n">
-        <v>0.02266</v>
+        <v>0.35754</v>
       </c>
       <c r="E156" t="n">
-        <v>0.00283</v>
+        <v>0.04469</v>
       </c>
       <c r="F156" t="n">
-        <v>0.23362</v>
+        <v>10.72041</v>
       </c>
       <c r="G156" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H156" t="n">
         <v>14</v>
@@ -4513,19 +4513,19 @@
         <v>1</v>
       </c>
       <c r="C157" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D157" t="n">
-        <v>0.02034</v>
+        <v>0.27414</v>
       </c>
       <c r="E157" t="n">
-        <v>0.00254</v>
+        <v>0.03427</v>
       </c>
       <c r="F157" t="n">
-        <v>0.1901</v>
+        <v>5.3212</v>
       </c>
       <c r="G157" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H157" t="n">
         <v>15</v>
@@ -4539,19 +4539,19 @@
         <v>1</v>
       </c>
       <c r="C158" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D158" t="n">
-        <v>0.01908</v>
+        <v>0.33132</v>
       </c>
       <c r="E158" t="n">
-        <v>0.00238</v>
+        <v>0.04142</v>
       </c>
       <c r="F158" t="n">
-        <v>0.21487</v>
+        <v>6.87457</v>
       </c>
       <c r="G158" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H158" t="n">
         <v>16</v>
@@ -4568,16 +4568,16 @@
         <v>11</v>
       </c>
       <c r="D159" t="n">
-        <v>0.01873</v>
+        <v>0.39722</v>
       </c>
       <c r="E159" t="n">
-        <v>0.00234</v>
+        <v>0.04965</v>
       </c>
       <c r="F159" t="n">
-        <v>0.2101</v>
+        <v>6.66531</v>
       </c>
       <c r="G159" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H159" t="n">
         <v>17</v>
@@ -4591,19 +4591,19 @@
         <v>1</v>
       </c>
       <c r="C160" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D160" t="n">
-        <v>0.02523</v>
+        <v>0.38027</v>
       </c>
       <c r="E160" t="n">
-        <v>0.00315</v>
+        <v>0.04753</v>
       </c>
       <c r="F160" t="n">
-        <v>0.23356</v>
+        <v>6.86945</v>
       </c>
       <c r="G160" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H160" t="n">
         <v>18</v>
@@ -4617,19 +4617,19 @@
         <v>1</v>
       </c>
       <c r="C161" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D161" t="n">
-        <v>0.01739</v>
+        <v>0.37056</v>
       </c>
       <c r="E161" t="n">
-        <v>0.00217</v>
+        <v>0.04632</v>
       </c>
       <c r="F161" t="n">
-        <v>0.21476</v>
+        <v>8.128819999999999</v>
       </c>
       <c r="G161" t="n">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="H161" t="n">
         <v>19</v>
@@ -4643,16 +4643,16 @@
         <v>1</v>
       </c>
       <c r="C162" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D162" t="n">
-        <v>0.01462</v>
+        <v>0.47906</v>
       </c>
       <c r="E162" t="n">
-        <v>0.00146</v>
+        <v>0.04791</v>
       </c>
       <c r="F162" t="n">
-        <v>0.14054</v>
+        <v>8.126139999999999</v>
       </c>
       <c r="G162" t="n">
         <v>0.85</v>
@@ -4669,16 +4669,16 @@
         <v>1</v>
       </c>
       <c r="C163" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D163" t="n">
-        <v>0.01544</v>
+        <v>0.46378</v>
       </c>
       <c r="E163" t="n">
-        <v>0.00154</v>
+        <v>0.04638</v>
       </c>
       <c r="F163" t="n">
-        <v>0.19223</v>
+        <v>7.23448</v>
       </c>
       <c r="G163" t="n">
         <v>0.85</v>
@@ -4695,16 +4695,16 @@
         <v>1</v>
       </c>
       <c r="C164" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D164" t="n">
-        <v>0.02188</v>
+        <v>0.29052</v>
       </c>
       <c r="E164" t="n">
-        <v>0.00219</v>
+        <v>0.02905</v>
       </c>
       <c r="F164" t="n">
-        <v>0.24671</v>
+        <v>5.88716</v>
       </c>
       <c r="G164" t="n">
         <v>0.85</v>
@@ -4721,16 +4721,16 @@
         <v>1</v>
       </c>
       <c r="C165" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D165" t="n">
-        <v>0.02152</v>
+        <v>0.29793</v>
       </c>
       <c r="E165" t="n">
-        <v>0.00215</v>
+        <v>0.02979</v>
       </c>
       <c r="F165" t="n">
-        <v>0.30289</v>
+        <v>6.14584</v>
       </c>
       <c r="G165" t="n">
         <v>0.85</v>
@@ -4747,16 +4747,16 @@
         <v>1</v>
       </c>
       <c r="C166" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D166" t="n">
-        <v>0.01778</v>
+        <v>0.31545</v>
       </c>
       <c r="E166" t="n">
-        <v>0.00178</v>
+        <v>0.03154</v>
       </c>
       <c r="F166" t="n">
-        <v>0.23817</v>
+        <v>4.54</v>
       </c>
       <c r="G166" t="n">
         <v>0.85</v>
@@ -4773,16 +4773,16 @@
         <v>1</v>
       </c>
       <c r="C167" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D167" t="n">
-        <v>0.01665</v>
+        <v>0.6423</v>
       </c>
       <c r="E167" t="n">
-        <v>0.00167</v>
+        <v>0.06423</v>
       </c>
       <c r="F167" t="n">
-        <v>0.27077</v>
+        <v>9.19487</v>
       </c>
       <c r="G167" t="n">
         <v>0.85</v>
@@ -4799,16 +4799,16 @@
         <v>1</v>
       </c>
       <c r="C168" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D168" t="n">
-        <v>0.02407</v>
+        <v>0.40292</v>
       </c>
       <c r="E168" t="n">
-        <v>0.00241</v>
+        <v>0.04029</v>
       </c>
       <c r="F168" t="n">
-        <v>0.34891</v>
+        <v>5.56912</v>
       </c>
       <c r="G168" t="n">
         <v>0.85</v>
@@ -4825,16 +4825,16 @@
         <v>1</v>
       </c>
       <c r="C169" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D169" t="n">
-        <v>0.01558</v>
+        <v>0.31121</v>
       </c>
       <c r="E169" t="n">
-        <v>0.00156</v>
+        <v>0.03112</v>
       </c>
       <c r="F169" t="n">
-        <v>0.2231</v>
+        <v>6.2185</v>
       </c>
       <c r="G169" t="n">
         <v>0.85</v>
@@ -4851,16 +4851,16 @@
         <v>1</v>
       </c>
       <c r="C170" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D170" t="n">
-        <v>0.01535</v>
+        <v>0.46569</v>
       </c>
       <c r="E170" t="n">
-        <v>0.00154</v>
+        <v>0.04657</v>
       </c>
       <c r="F170" t="n">
-        <v>0.16354</v>
+        <v>12.16796</v>
       </c>
       <c r="G170" t="n">
         <v>0.85</v>
@@ -4877,16 +4877,16 @@
         <v>1</v>
       </c>
       <c r="C171" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D171" t="n">
-        <v>0.01182</v>
+        <v>0.48764</v>
       </c>
       <c r="E171" t="n">
-        <v>0.00118</v>
+        <v>0.04876</v>
       </c>
       <c r="F171" t="n">
-        <v>0.15984</v>
+        <v>6.95835</v>
       </c>
       <c r="G171" t="n">
         <v>0.85</v>
@@ -4903,16 +4903,16 @@
         <v>1</v>
       </c>
       <c r="C172" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D172" t="n">
-        <v>0.01208</v>
+        <v>0.70019</v>
       </c>
       <c r="E172" t="n">
-        <v>0.00121</v>
+        <v>0.07002</v>
       </c>
       <c r="F172" t="n">
-        <v>0.10264</v>
+        <v>9.13641</v>
       </c>
       <c r="G172" t="n">
         <v>0.85</v>
@@ -4929,16 +4929,16 @@
         <v>1</v>
       </c>
       <c r="C173" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D173" t="n">
-        <v>0.01316</v>
+        <v>0.24539</v>
       </c>
       <c r="E173" t="n">
-        <v>0.00132</v>
+        <v>0.02454</v>
       </c>
       <c r="F173" t="n">
-        <v>0.13619</v>
+        <v>4.96085</v>
       </c>
       <c r="G173" t="n">
         <v>0.85</v>
@@ -4955,16 +4955,16 @@
         <v>1</v>
       </c>
       <c r="C174" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D174" t="n">
-        <v>0.01175</v>
+        <v>0.39556</v>
       </c>
       <c r="E174" t="n">
-        <v>0.00118</v>
+        <v>0.03956</v>
       </c>
       <c r="F174" t="n">
-        <v>0.12455</v>
+        <v>6.99905</v>
       </c>
       <c r="G174" t="n">
         <v>0.85</v>
@@ -4981,16 +4981,16 @@
         <v>1</v>
       </c>
       <c r="C175" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D175" t="n">
-        <v>0.01629</v>
+        <v>0.32487</v>
       </c>
       <c r="E175" t="n">
-        <v>0.00163</v>
+        <v>0.03249</v>
       </c>
       <c r="F175" t="n">
-        <v>0.1682</v>
+        <v>7.00838</v>
       </c>
       <c r="G175" t="n">
         <v>0.85</v>
@@ -5007,16 +5007,16 @@
         <v>1</v>
       </c>
       <c r="C176" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D176" t="n">
-        <v>0.02206</v>
+        <v>0.23215</v>
       </c>
       <c r="E176" t="n">
-        <v>0.00221</v>
+        <v>0.02321</v>
       </c>
       <c r="F176" t="n">
-        <v>0.27267</v>
+        <v>4.45307</v>
       </c>
       <c r="G176" t="n">
         <v>0.85</v>
@@ -5036,13 +5036,13 @@
         <v>9</v>
       </c>
       <c r="D177" t="n">
-        <v>0.01039</v>
+        <v>0.35365</v>
       </c>
       <c r="E177" t="n">
-        <v>0.00104</v>
+        <v>0.03537</v>
       </c>
       <c r="F177" t="n">
-        <v>0.09852</v>
+        <v>5.03827</v>
       </c>
       <c r="G177" t="n">
         <v>0.85</v>
@@ -5059,16 +5059,16 @@
         <v>1</v>
       </c>
       <c r="C178" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D178" t="n">
-        <v>0.01638</v>
+        <v>0.80443</v>
       </c>
       <c r="E178" t="n">
-        <v>0.00164</v>
+        <v>0.08044</v>
       </c>
       <c r="F178" t="n">
-        <v>0.18819</v>
+        <v>12.9368</v>
       </c>
       <c r="G178" t="n">
         <v>0.85</v>
@@ -5085,16 +5085,16 @@
         <v>1</v>
       </c>
       <c r="C179" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D179" t="n">
-        <v>0.01264</v>
+        <v>0.32199</v>
       </c>
       <c r="E179" t="n">
-        <v>0.00126</v>
+        <v>0.0322</v>
       </c>
       <c r="F179" t="n">
-        <v>0.15962</v>
+        <v>7.34225</v>
       </c>
       <c r="G179" t="n">
         <v>0.85</v>
@@ -5114,13 +5114,13 @@
         <v>17</v>
       </c>
       <c r="D180" t="n">
-        <v>0.01691</v>
+        <v>0.43627</v>
       </c>
       <c r="E180" t="n">
-        <v>0.00169</v>
+        <v>0.04363</v>
       </c>
       <c r="F180" t="n">
-        <v>0.29452</v>
+        <v>10.27768</v>
       </c>
       <c r="G180" t="n">
         <v>0.85</v>
@@ -5137,16 +5137,16 @@
         <v>1</v>
       </c>
       <c r="C181" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D181" t="n">
-        <v>0.01191</v>
+        <v>0.46358</v>
       </c>
       <c r="E181" t="n">
-        <v>0.00119</v>
+        <v>0.04636</v>
       </c>
       <c r="F181" t="n">
-        <v>0.13706</v>
+        <v>8.90448</v>
       </c>
       <c r="G181" t="n">
         <v>0.85</v>
@@ -5163,16 +5163,16 @@
         <v>1</v>
       </c>
       <c r="C182" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D182" t="n">
-        <v>0.02869</v>
+        <v>0.6494799999999999</v>
       </c>
       <c r="E182" t="n">
-        <v>0.00287</v>
+        <v>0.06494999999999999</v>
       </c>
       <c r="F182" t="n">
-        <v>0.18014</v>
+        <v>7.35053</v>
       </c>
       <c r="G182" t="n">
         <v>0.15</v>
@@ -5192,13 +5192,13 @@
         <v>9</v>
       </c>
       <c r="D183" t="n">
-        <v>0.0247</v>
+        <v>1.32606</v>
       </c>
       <c r="E183" t="n">
-        <v>0.00247</v>
+        <v>0.13261</v>
       </c>
       <c r="F183" t="n">
-        <v>0.23087</v>
+        <v>16.43853</v>
       </c>
       <c r="G183" t="n">
         <v>0.15</v>
@@ -5215,16 +5215,16 @@
         <v>1</v>
       </c>
       <c r="C184" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D184" t="n">
-        <v>0.02493</v>
+        <v>0.54236</v>
       </c>
       <c r="E184" t="n">
-        <v>0.00249</v>
+        <v>0.05424</v>
       </c>
       <c r="F184" t="n">
-        <v>0.18152</v>
+        <v>9.083259999999999</v>
       </c>
       <c r="G184" t="n">
         <v>0.15</v>
@@ -5244,13 +5244,13 @@
         <v>7</v>
       </c>
       <c r="D185" t="n">
-        <v>0.0225</v>
+        <v>0.59317</v>
       </c>
       <c r="E185" t="n">
-        <v>0.00225</v>
+        <v>0.05932</v>
       </c>
       <c r="F185" t="n">
-        <v>0.16552</v>
+        <v>7.18133</v>
       </c>
       <c r="G185" t="n">
         <v>0.15</v>
@@ -5267,16 +5267,16 @@
         <v>1</v>
       </c>
       <c r="C186" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D186" t="n">
-        <v>0.025</v>
+        <v>0.8974299999999999</v>
       </c>
       <c r="E186" t="n">
-        <v>0.0025</v>
+        <v>0.08974</v>
       </c>
       <c r="F186" t="n">
-        <v>0.23101</v>
+        <v>8.97017</v>
       </c>
       <c r="G186" t="n">
         <v>0.15</v>
@@ -5293,16 +5293,16 @@
         <v>1</v>
       </c>
       <c r="C187" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D187" t="n">
-        <v>0.02601</v>
+        <v>0.53029</v>
       </c>
       <c r="E187" t="n">
-        <v>0.0026</v>
+        <v>0.05303</v>
       </c>
       <c r="F187" t="n">
-        <v>0.26527</v>
+        <v>10.42959</v>
       </c>
       <c r="G187" t="n">
         <v>0.15</v>
@@ -5319,16 +5319,16 @@
         <v>1</v>
       </c>
       <c r="C188" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D188" t="n">
-        <v>0.02121</v>
+        <v>0.64569</v>
       </c>
       <c r="E188" t="n">
-        <v>0.00212</v>
+        <v>0.06457</v>
       </c>
       <c r="F188" t="n">
-        <v>0.11703</v>
+        <v>9.21453</v>
       </c>
       <c r="G188" t="n">
         <v>0.15</v>
@@ -5345,16 +5345,16 @@
         <v>1</v>
       </c>
       <c r="C189" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D189" t="n">
-        <v>0.01752</v>
+        <v>0.47697</v>
       </c>
       <c r="E189" t="n">
-        <v>0.00175</v>
+        <v>0.0477</v>
       </c>
       <c r="F189" t="n">
-        <v>0.09358</v>
+        <v>4.85772</v>
       </c>
       <c r="G189" t="n">
         <v>0.15</v>
@@ -5371,16 +5371,16 @@
         <v>1</v>
       </c>
       <c r="C190" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D190" t="n">
-        <v>0.02237</v>
+        <v>0.36444</v>
       </c>
       <c r="E190" t="n">
-        <v>0.00224</v>
+        <v>0.03644</v>
       </c>
       <c r="F190" t="n">
-        <v>0.1636</v>
+        <v>4.7403</v>
       </c>
       <c r="G190" t="n">
         <v>0.15</v>
@@ -5397,16 +5397,16 @@
         <v>1</v>
       </c>
       <c r="C191" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D191" t="n">
-        <v>0.01968</v>
+        <v>0.21476</v>
       </c>
       <c r="E191" t="n">
-        <v>0.00197</v>
+        <v>0.02148</v>
       </c>
       <c r="F191" t="n">
-        <v>0.14576</v>
+        <v>4.65366</v>
       </c>
       <c r="G191" t="n">
         <v>0.15</v>
@@ -5423,16 +5423,16 @@
         <v>1</v>
       </c>
       <c r="C192" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D192" t="n">
-        <v>0.02787</v>
+        <v>0.37998</v>
       </c>
       <c r="E192" t="n">
-        <v>0.00279</v>
+        <v>0.038</v>
       </c>
       <c r="F192" t="n">
-        <v>0.20117</v>
+        <v>6.10015</v>
       </c>
       <c r="G192" t="n">
         <v>0.15</v>
@@ -5449,16 +5449,16 @@
         <v>1</v>
       </c>
       <c r="C193" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D193" t="n">
-        <v>0.02301</v>
+        <v>0.3748</v>
       </c>
       <c r="E193" t="n">
-        <v>0.0023</v>
+        <v>0.03748</v>
       </c>
       <c r="F193" t="n">
-        <v>0.19311</v>
+        <v>5.0176</v>
       </c>
       <c r="G193" t="n">
         <v>0.15</v>
@@ -5475,16 +5475,16 @@
         <v>1</v>
       </c>
       <c r="C194" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D194" t="n">
-        <v>0.02629</v>
+        <v>0.51164</v>
       </c>
       <c r="E194" t="n">
-        <v>0.00263</v>
+        <v>0.05116</v>
       </c>
       <c r="F194" t="n">
-        <v>0.24257</v>
+        <v>4.98977</v>
       </c>
       <c r="G194" t="n">
         <v>0.15</v>
@@ -5501,16 +5501,16 @@
         <v>1</v>
       </c>
       <c r="C195" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D195" t="n">
-        <v>0.02477</v>
+        <v>0.50656</v>
       </c>
       <c r="E195" t="n">
-        <v>0.00248</v>
+        <v>0.05066</v>
       </c>
       <c r="F195" t="n">
-        <v>0.25369</v>
+        <v>3.88826</v>
       </c>
       <c r="G195" t="n">
         <v>0.15</v>
@@ -5527,16 +5527,16 @@
         <v>1</v>
       </c>
       <c r="C196" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D196" t="n">
-        <v>0.01259</v>
+        <v>0.56591</v>
       </c>
       <c r="E196" t="n">
-        <v>0.00126</v>
+        <v>0.05659</v>
       </c>
       <c r="F196" t="n">
-        <v>0.08456</v>
+        <v>9.564870000000001</v>
       </c>
       <c r="G196" t="n">
         <v>0.15</v>
@@ -5553,16 +5553,16 @@
         <v>1</v>
       </c>
       <c r="C197" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D197" t="n">
-        <v>0.01916</v>
+        <v>0.56093</v>
       </c>
       <c r="E197" t="n">
-        <v>0.00192</v>
+        <v>0.05609</v>
       </c>
       <c r="F197" t="n">
-        <v>0.13915</v>
+        <v>4.60574</v>
       </c>
       <c r="G197" t="n">
         <v>0.15</v>
@@ -5579,16 +5579,16 @@
         <v>1</v>
       </c>
       <c r="C198" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D198" t="n">
-        <v>0.0128</v>
+        <v>0.43766</v>
       </c>
       <c r="E198" t="n">
-        <v>0.00128</v>
+        <v>0.04377</v>
       </c>
       <c r="F198" t="n">
-        <v>0.06901</v>
+        <v>5.80792</v>
       </c>
       <c r="G198" t="n">
         <v>0.15</v>
@@ -5605,16 +5605,16 @@
         <v>1</v>
       </c>
       <c r="C199" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D199" t="n">
-        <v>0.02816</v>
+        <v>0.54567</v>
       </c>
       <c r="E199" t="n">
-        <v>0.00282</v>
+        <v>0.05457</v>
       </c>
       <c r="F199" t="n">
-        <v>0.26047</v>
+        <v>6.22216</v>
       </c>
       <c r="G199" t="n">
         <v>0.15</v>
@@ -5631,16 +5631,16 @@
         <v>1</v>
       </c>
       <c r="C200" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D200" t="n">
-        <v>0.01987</v>
+        <v>0.47793</v>
       </c>
       <c r="E200" t="n">
-        <v>0.00199</v>
+        <v>0.04779</v>
       </c>
       <c r="F200" t="n">
-        <v>0.12423</v>
+        <v>7.21443</v>
       </c>
       <c r="G200" t="n">
         <v>0.15</v>
@@ -5657,16 +5657,16 @@
         <v>1</v>
       </c>
       <c r="C201" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D201" t="n">
-        <v>0.02485</v>
+        <v>0.45149</v>
       </c>
       <c r="E201" t="n">
-        <v>0.00249</v>
+        <v>0.04515</v>
       </c>
       <c r="F201" t="n">
-        <v>0.22965</v>
+        <v>7.48461</v>
       </c>
       <c r="G201" t="n">
         <v>0.15</v>

</xml_diff>